<commit_message>
- sửa lỗi chính tả, merge của Bình vào
</commit_message>
<xml_diff>
--- a/5th Week/MockProcject_Database Design.xlsx
+++ b/5th Week/MockProcject_Database Design.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\001_IT BOOK\Nam 4\2. Ky II\Do an CNPM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\001_IT BOOK\Nam 4\2. Ky II\Do an CNPM\[DO AN] Nhom Chanh, Binh, Dung, Cung\5th Week\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="61">
   <si>
     <t>Maxlength</t>
     <phoneticPr fontId="0"/>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>TimeBookId</t>
+  </si>
+  <si>
+    <t>UserRole = {Admin, Staff}</t>
   </si>
 </sst>
 </file>
@@ -297,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -314,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,9 +859,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -870,8 +876,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2362200" y="838200"/>
-          <a:ext cx="476250" cy="3057525"/>
+          <a:off x="1838325" y="838201"/>
+          <a:ext cx="619125" cy="3057524"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1210,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I26"/>
+  <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,12 +1548,12 @@
     <col min="16134" max="16134" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1558,7 +1564,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1588,8 +1594,11 @@
       <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1603,7 +1612,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1617,7 +1626,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>4</v>
       </c>
@@ -1645,7 +1654,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
         <v>26</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
@@ -1667,24 +1676,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="12" t="s">
         <v>45</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D13" s="7"/>
       <c r="G13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1698,7 +1707,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1816,7 +1825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
! done SE18_SRS_v3.0.doc and Mocking DB
</commit_message>
<xml_diff>
--- a/5th Week/MockProcject_Database Design.xlsx
+++ b/5th Week/MockProcject_Database Design.xlsx
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,14 @@
       <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -300,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -320,6 +328,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,7 +1588,7 @@
       <c r="H4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1628,7 +1638,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -1645,7 +1655,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -1746,10 +1756,10 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1765,10 +1775,10 @@
       <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1778,12 +1788,12 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="14" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1804,7 +1814,7 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -1826,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1889,7 +1899,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1901,7 +1911,7 @@
       <c r="D3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1913,7 +1923,7 @@
       <c r="I3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -1972,7 +1982,7 @@
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1992,7 +2002,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2040,7 +2050,7 @@
         <v>50</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -2052,7 +2062,7 @@
       <c r="I8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -2130,7 +2140,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -2142,7 +2152,7 @@
       <c r="I14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L14" s="3" t="s">
@@ -2275,7 +2285,7 @@
         <v>50</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="13" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -2287,7 +2297,7 @@
       <c r="I21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="L21" s="3" t="s">
@@ -2319,7 +2329,7 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="14" t="s">
         <v>7</v>
       </c>
       <c r="L22" s="3" t="s">
@@ -2407,7 +2417,7 @@
       </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="14" t="s">
         <v>29</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -2553,7 +2563,7 @@
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2565,7 +2575,7 @@
       <c r="D36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="14" t="s">
         <v>29</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -2597,7 +2607,7 @@
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2609,7 +2619,7 @@
       <c r="D38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="14" t="s">
         <v>18</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -2624,5 +2634,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>